<commit_message>
Interpolation for missing data Not completed
</commit_message>
<xml_diff>
--- a/Travel_data_full_column.xlsx
+++ b/Travel_data_full_column.xlsx
@@ -342,7 +342,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
@@ -369,19 +369,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -426,7 +413,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -435,16 +422,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -467,7 +446,7 @@
   <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,7 +460,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.08"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,21 +488,21 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -547,24 +526,24 @@
       <c r="I2" s="0" t="n">
         <v>2495438</v>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="J2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -588,24 +567,24 @@
       <c r="I3" s="0" t="n">
         <v>2657800</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="M3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -629,24 +608,24 @@
       <c r="I4" s="0" t="n">
         <v>2465821</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="M4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -670,24 +649,24 @@
       <c r="I5" s="0" t="n">
         <v>2687229</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -711,24 +690,24 @@
       <c r="I6" s="0" t="n">
         <v>2669854</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -752,24 +731,24 @@
       <c r="I7" s="0" t="n">
         <v>2644596</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="M7" s="4" t="n">
+      <c r="M7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -793,24 +772,24 @@
       <c r="I8" s="0" t="n">
         <v>2388222</v>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L8" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="M8" s="4" t="n">
+      <c r="M8" s="1" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -834,24 +813,24 @@
       <c r="I9" s="0" t="n">
         <v>2404130</v>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L9" s="4" t="n">
+      <c r="L9" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="M9" s="4" t="n">
+      <c r="M9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -875,24 +854,24 @@
       <c r="I10" s="0" t="n">
         <v>2477908</v>
       </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="K10" s="4" t="n">
+      <c r="K10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="L10" s="4" t="n">
+      <c r="L10" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="M10" s="1" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -916,24 +895,24 @@
       <c r="I11" s="0" t="n">
         <v>2158770</v>
       </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="K11" s="4" t="n">
+      <c r="K11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="L11" s="4" t="n">
+      <c r="L11" s="1" t="n">
         <v>281</v>
       </c>
-      <c r="M11" s="4" t="n">
+      <c r="M11" s="1" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -957,24 +936,24 @@
       <c r="I12" s="0" t="n">
         <v>2525320</v>
       </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="1" t="n">
         <v>205</v>
       </c>
-      <c r="K12" s="4" t="n">
+      <c r="K12" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="L12" s="4" t="n">
+      <c r="L12" s="1" t="n">
         <v>427</v>
       </c>
-      <c r="M12" s="4" t="n">
+      <c r="M12" s="1" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -998,24 +977,24 @@
       <c r="I13" s="0" t="n">
         <v>2477879</v>
       </c>
-      <c r="J13" s="4" t="n">
+      <c r="J13" s="1" t="n">
         <v>385</v>
       </c>
-      <c r="K13" s="4" t="n">
+      <c r="K13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="L13" s="4" t="n">
+      <c r="L13" s="1" t="n">
         <v>749</v>
       </c>
-      <c r="M13" s="4" t="n">
+      <c r="M13" s="1" t="n">
         <v>52</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -1039,24 +1018,24 @@
       <c r="I14" s="0" t="n">
         <v>2432398</v>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="1" t="n">
         <v>523</v>
       </c>
-      <c r="K14" s="4" t="n">
+      <c r="K14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="L14" s="4" t="n">
+      <c r="L14" s="1" t="n">
         <v>1144</v>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="M14" s="1" t="n">
         <v>116</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -1080,24 +1059,24 @@
       <c r="I15" s="0" t="n">
         <v>2430787</v>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="1" t="n">
         <v>835</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" s="1" t="n">
         <v>1824</v>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="M15" s="1" t="n">
         <v>144</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -1121,24 +1100,24 @@
       <c r="I16" s="0" t="n">
         <v>2504218</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="1" t="n">
         <v>586</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="L16" s="4" t="n">
+      <c r="L16" s="1" t="n">
         <v>2278</v>
       </c>
-      <c r="M16" s="4" t="n">
+      <c r="M16" s="1" t="n">
         <v>117</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -1162,24 +1141,24 @@
       <c r="I17" s="0" t="n">
         <v>2427394</v>
       </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="1" t="n">
         <v>591</v>
       </c>
-      <c r="K17" s="4" t="n">
+      <c r="K17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="L17" s="4" t="n">
+      <c r="L17" s="1" t="n">
         <v>2666</v>
       </c>
-      <c r="M17" s="4" t="n">
+      <c r="M17" s="1" t="n">
         <v>187</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -1203,24 +1182,24 @@
       <c r="I18" s="0" t="n">
         <v>1983450</v>
       </c>
-      <c r="J18" s="4" t="n">
+      <c r="J18" s="1" t="n">
         <v>1234</v>
       </c>
-      <c r="K18" s="4" t="n">
+      <c r="K18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="L18" s="4" t="n">
+      <c r="L18" s="1" t="n">
         <v>3710</v>
       </c>
-      <c r="M18" s="4" t="n">
+      <c r="M18" s="1" t="n">
         <v>174</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -1244,24 +1223,24 @@
       <c r="I19" s="0" t="n">
         <v>2367141</v>
       </c>
-      <c r="J19" s="4" t="n">
+      <c r="J19" s="1" t="n">
         <v>1076</v>
       </c>
-      <c r="K19" s="4" t="n">
+      <c r="K19" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="L19" s="4" t="n">
+      <c r="L19" s="1" t="n">
         <v>4009</v>
       </c>
-      <c r="M19" s="4" t="n">
+      <c r="M19" s="1" t="n">
         <v>756</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -1285,24 +1264,24 @@
       <c r="I20" s="0" t="n">
         <v>2000405</v>
       </c>
-      <c r="J20" s="4" t="n">
+      <c r="J20" s="1" t="n">
         <v>743</v>
       </c>
-      <c r="K20" s="4" t="n">
+      <c r="K20" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="L20" s="4" t="n">
+      <c r="L20" s="1" t="n">
         <v>4238</v>
       </c>
-      <c r="M20" s="4" t="n">
+      <c r="M20" s="1" t="n">
         <v>465</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -1326,24 +1305,24 @@
       <c r="I21" s="0" t="n">
         <v>2391281</v>
       </c>
-      <c r="J21" s="4" t="n">
+      <c r="J21" s="1" t="n">
         <v>595</v>
       </c>
-      <c r="K21" s="4" t="n">
+      <c r="K21" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="L21" s="4" t="n">
+      <c r="L21" s="1" t="n">
         <v>4530</v>
       </c>
-      <c r="M21" s="4" t="n">
+      <c r="M21" s="1" t="n">
         <v>260</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -1367,24 +1346,24 @@
       <c r="I22" s="0" t="n">
         <v>2329436</v>
       </c>
-      <c r="J22" s="4" t="n">
+      <c r="J22" s="1" t="n">
         <v>881</v>
       </c>
-      <c r="K22" s="4" t="n">
+      <c r="K22" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="L22" s="4" t="n">
+      <c r="L22" s="1" t="n">
         <v>5020</v>
       </c>
-      <c r="M22" s="4" t="n">
+      <c r="M22" s="1" t="n">
         <v>337</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -1408,24 +1387,24 @@
       <c r="I23" s="0" t="n">
         <v>2353970</v>
       </c>
-      <c r="J23" s="4" t="n">
+      <c r="J23" s="1" t="n">
         <v>958</v>
       </c>
-      <c r="K23" s="4" t="n">
+      <c r="K23" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="L23" s="4" t="n">
+      <c r="L23" s="1" t="n">
         <v>5687</v>
       </c>
-      <c r="M23" s="4" t="n">
+      <c r="M23" s="1" t="n">
         <v>228</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -1449,24 +1428,24 @@
       <c r="I24" s="0" t="n">
         <v>2235659</v>
       </c>
-      <c r="J24" s="4" t="n">
+      <c r="J24" s="1" t="n">
         <v>1075</v>
       </c>
-      <c r="K24" s="4" t="n">
+      <c r="K24" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="L24" s="4" t="n">
+      <c r="L24" s="1" t="n">
         <v>6370</v>
       </c>
-      <c r="M24" s="4" t="n">
+      <c r="M24" s="1" t="n">
         <v>317</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -1490,24 +1469,24 @@
       <c r="I25" s="0" t="n">
         <v>1766662</v>
       </c>
-      <c r="J25" s="4" t="n">
+      <c r="J25" s="1" t="n">
         <v>1289</v>
       </c>
-      <c r="K25" s="4" t="n">
+      <c r="K25" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="L25" s="4" t="n">
+      <c r="L25" s="1" t="n">
         <v>7321</v>
       </c>
-      <c r="M25" s="4" t="n">
+      <c r="M25" s="1" t="n">
         <v>253</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -1531,24 +1510,24 @@
       <c r="I26" s="0" t="n">
         <v>2403525</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="1" t="n">
         <v>1365</v>
       </c>
-      <c r="K26" s="4" t="n">
+      <c r="K26" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="L26" s="4" t="n">
+      <c r="L26" s="1" t="n">
         <v>7779</v>
       </c>
-      <c r="M26" s="4" t="n">
+      <c r="M26" s="1" t="n">
         <v>810</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -1572,24 +1551,24 @@
       <c r="I27" s="0" t="n">
         <v>2350691</v>
       </c>
-      <c r="J27" s="4" t="n">
+      <c r="J27" s="1" t="n">
         <v>1209</v>
       </c>
-      <c r="K27" s="4" t="n">
+      <c r="K27" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="L27" s="4" t="n">
+      <c r="L27" s="1" t="n">
         <v>8624</v>
       </c>
-      <c r="M27" s="4" t="n">
+      <c r="M27" s="1" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="0" t="n">
@@ -1613,24 +1592,24 @@
       <c r="I28" s="0" t="n">
         <v>2335525</v>
       </c>
-      <c r="J28" s="4" t="n">
+      <c r="J28" s="1" t="n">
         <v>1053</v>
       </c>
-      <c r="K28" s="4" t="n">
+      <c r="K28" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="L28" s="4" t="n">
+      <c r="L28" s="1" t="n">
         <v>9142</v>
       </c>
-      <c r="M28" s="4" t="n">
+      <c r="M28" s="1" t="n">
         <v>406</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -1654,24 +1633,24 @@
       <c r="I29" s="0" t="n">
         <v>2193148</v>
       </c>
-      <c r="J29" s="4" t="n">
+      <c r="J29" s="1" t="n">
         <v>1178</v>
       </c>
-      <c r="K29" s="4" t="n">
+      <c r="K29" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="L29" s="4" t="n">
+      <c r="L29" s="1" t="n">
         <v>9792</v>
       </c>
-      <c r="M29" s="4" t="n">
+      <c r="M29" s="1" t="n">
         <v>393</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -1695,24 +1674,24 @@
       <c r="I30" s="0" t="n">
         <v>2055656</v>
       </c>
-      <c r="J30" s="4" t="n">
+      <c r="J30" s="1" t="n">
         <v>1192</v>
       </c>
-      <c r="K30" s="4" t="n">
+      <c r="K30" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="L30" s="4" t="n">
+      <c r="L30" s="1" t="n">
         <v>10516</v>
       </c>
-      <c r="M30" s="4" t="n">
+      <c r="M30" s="1" t="n">
         <v>321</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -1736,24 +1715,24 @@
       <c r="I31" s="0" t="n">
         <v>1632769</v>
       </c>
-      <c r="J31" s="4" t="n">
+      <c r="J31" s="1" t="n">
         <v>1046</v>
       </c>
-      <c r="K31" s="4" t="n">
+      <c r="K31" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="L31" s="4" t="n">
+      <c r="L31" s="1" t="n">
         <v>11144</v>
       </c>
-      <c r="M31" s="4" t="n">
+      <c r="M31" s="1" t="n">
         <v>269</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -1777,24 +1756,24 @@
       <c r="I32" s="0" t="n">
         <v>1118333</v>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="1" t="n">
         <v>1237</v>
       </c>
-      <c r="K32" s="4" t="n">
+      <c r="K32" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="L32" s="4" t="n">
+      <c r="L32" s="1" t="n">
         <v>11466</v>
       </c>
-      <c r="M32" s="4" t="n">
+      <c r="M32" s="1" t="n">
         <v>766</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="0" t="n">
@@ -1818,24 +1797,24 @@
       <c r="I33" s="0" t="n">
         <v>1275236</v>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="1" t="n">
         <v>966</v>
       </c>
-      <c r="K33" s="4" t="n">
+      <c r="K33" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="L33" s="4" t="n">
+      <c r="L33" s="1" t="n">
         <v>11419</v>
       </c>
-      <c r="M33" s="4" t="n">
+      <c r="M33" s="1" t="n">
         <v>890</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="0" t="n">
@@ -1859,24 +1838,24 @@
       <c r="I34" s="0" t="n">
         <v>1214278</v>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="1" t="n">
         <v>1028</v>
       </c>
-      <c r="K34" s="4" t="n">
+      <c r="K34" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="L34" s="4" t="n">
+      <c r="L34" s="1" t="n">
         <v>12040</v>
       </c>
-      <c r="M34" s="4" t="n">
+      <c r="M34" s="1" t="n">
         <v>278</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="0" t="n">
@@ -1900,24 +1879,24 @@
       <c r="I35" s="0" t="n">
         <v>1205309</v>
       </c>
-      <c r="J35" s="4" t="n">
+      <c r="J35" s="1" t="n">
         <v>1411</v>
       </c>
-      <c r="K35" s="4" t="n">
+      <c r="K35" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="L35" s="4" t="n">
+      <c r="L35" s="1" t="n">
         <v>12861</v>
       </c>
-      <c r="M35" s="4" t="n">
+      <c r="M35" s="1" t="n">
         <v>463</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C36" s="0" t="n">
@@ -1941,24 +1920,24 @@
       <c r="I36" s="0" t="n">
         <v>1441438</v>
       </c>
-      <c r="J36" s="4" t="n">
+      <c r="J36" s="1" t="n">
         <v>1762</v>
       </c>
-      <c r="K36" s="4" t="n">
+      <c r="K36" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="L36" s="4" t="n">
+      <c r="L36" s="1" t="n">
         <v>13964</v>
       </c>
-      <c r="M36" s="4" t="n">
+      <c r="M36" s="1" t="n">
         <v>537</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -1982,24 +1961,24 @@
       <c r="I37" s="0" t="n">
         <v>1505018</v>
       </c>
-      <c r="J37" s="4" t="n">
+      <c r="J37" s="1" t="n">
         <v>2206</v>
       </c>
-      <c r="K37" s="4" t="n">
+      <c r="K37" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="L37" s="4" t="n">
+      <c r="L37" s="1" t="n">
         <v>15315</v>
       </c>
-      <c r="M37" s="4" t="n">
+      <c r="M37" s="1" t="n">
         <v>712</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="0" t="n">
@@ -2023,24 +2002,24 @@
       <c r="I38" s="0" t="n">
         <v>1345962</v>
       </c>
-      <c r="J38" s="4" t="n">
+      <c r="J38" s="1" t="n">
         <v>2389</v>
       </c>
-      <c r="K38" s="4" t="n">
+      <c r="K38" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="L38" s="4" t="n">
+      <c r="L38" s="1" t="n">
         <v>16715</v>
       </c>
-      <c r="M38" s="4" t="n">
+      <c r="M38" s="1" t="n">
         <v>832</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -2064,24 +2043,24 @@
       <c r="I39" s="0" t="n">
         <v>1057012</v>
       </c>
-      <c r="J39" s="4" t="n">
+      <c r="J39" s="1" t="n">
         <v>2926</v>
       </c>
-      <c r="K39" s="4" t="n">
+      <c r="K39" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="L39" s="4" t="n">
+      <c r="L39" s="1" t="n">
         <v>18821</v>
       </c>
-      <c r="M39" s="4" t="n">
+      <c r="M39" s="1" t="n">
         <v>676</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="0" t="n">
@@ -2105,24 +2084,24 @@
       <c r="I40" s="0" t="n">
         <v>1190473</v>
       </c>
-      <c r="J40" s="4" t="n">
+      <c r="J40" s="1" t="n">
         <v>3076</v>
       </c>
-      <c r="K40" s="4" t="n">
+      <c r="K40" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="L40" s="4" t="n">
+      <c r="L40" s="1" t="n">
         <v>21212</v>
       </c>
-      <c r="M40" s="4" t="n">
+      <c r="M40" s="1" t="n">
         <v>546</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="0" t="n">
@@ -2146,24 +2125,24 @@
       <c r="I41" s="0" t="n">
         <v>1057221</v>
       </c>
-      <c r="J41" s="4" t="n">
+      <c r="J41" s="1" t="n">
         <v>2901</v>
       </c>
-      <c r="K41" s="4" t="n">
+      <c r="K41" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="L41" s="4" t="n">
+      <c r="L41" s="1" t="n">
         <v>23278</v>
       </c>
-      <c r="M41" s="4" t="n">
+      <c r="M41" s="1" t="n">
         <v>712</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C42" s="0" t="n">
@@ -2187,24 +2166,24 @@
       <c r="I42" s="0" t="n">
         <v>1124439</v>
       </c>
-      <c r="J42" s="4" t="n">
+      <c r="J42" s="1" t="n">
         <v>3186</v>
       </c>
-      <c r="K42" s="4" t="n">
+      <c r="K42" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="L42" s="4" t="n">
+      <c r="L42" s="1" t="n">
         <v>24827</v>
       </c>
-      <c r="M42" s="4" t="n">
+      <c r="M42" s="1" t="n">
         <v>1520</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="0" t="n">
@@ -2228,24 +2207,24 @@
       <c r="I43" s="0" t="n">
         <v>924337</v>
       </c>
-      <c r="J43" s="4" t="n">
+      <c r="J43" s="1" t="n">
         <v>3110</v>
       </c>
-      <c r="K43" s="4" t="n">
+      <c r="K43" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="L43" s="4" t="n">
+      <c r="L43" s="1" t="n">
         <v>27051</v>
       </c>
-      <c r="M43" s="4" t="n">
+      <c r="M43" s="1" t="n">
         <v>745</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C44" s="0" t="n">
@@ -2269,24 +2248,24 @@
       <c r="I44" s="0" t="n">
         <v>616968</v>
       </c>
-      <c r="J44" s="4" t="n">
+      <c r="J44" s="1" t="n">
         <v>2988</v>
       </c>
-      <c r="K44" s="4" t="n">
+      <c r="K44" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="L44" s="4" t="n">
+      <c r="L44" s="1" t="n">
         <v>29084</v>
       </c>
-      <c r="M44" s="4" t="n">
+      <c r="M44" s="1" t="n">
         <v>817</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="0" t="n">
@@ -2310,24 +2289,24 @@
       <c r="I45" s="0" t="n">
         <v>1136894</v>
       </c>
-      <c r="J45" s="4" t="n">
+      <c r="J45" s="1" t="n">
         <v>2875</v>
       </c>
-      <c r="K45" s="4" t="n">
+      <c r="K45" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="L45" s="4" t="n">
+      <c r="L45" s="1" t="n">
         <v>30597</v>
       </c>
-      <c r="M45" s="4" t="n">
+      <c r="M45" s="1" t="n">
         <v>1238</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>73</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C46" s="0" t="n">
@@ -2351,24 +2330,24 @@
       <c r="I46" s="0" t="n">
         <v>1103582</v>
       </c>
-      <c r="J46" s="4" t="n">
+      <c r="J46" s="1" t="n">
         <v>2715</v>
       </c>
-      <c r="K46" s="4" t="n">
+      <c r="K46" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="L46" s="4" t="n">
+      <c r="L46" s="1" t="n">
         <v>31954</v>
       </c>
-      <c r="M46" s="4" t="n">
+      <c r="M46" s="1" t="n">
         <v>1224</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C47" s="0" t="n">
@@ -2392,24 +2371,24 @@
       <c r="I47" s="0" t="n">
         <v>1563390</v>
       </c>
-      <c r="J47" s="4" t="n">
+      <c r="J47" s="1" t="n">
         <v>2560</v>
       </c>
-      <c r="K47" s="4" t="n">
+      <c r="K47" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="L47" s="4" t="n">
+      <c r="L47" s="1" t="n">
         <v>32555</v>
       </c>
-      <c r="M47" s="4" t="n">
+      <c r="M47" s="1" t="n">
         <v>1801</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C48" s="0" t="n">
@@ -2433,24 +2412,24 @@
       <c r="I48" s="0" t="n">
         <v>1551766</v>
       </c>
-      <c r="J48" s="4" t="n">
+      <c r="J48" s="1" t="n">
         <v>2483</v>
       </c>
-      <c r="K48" s="4" t="n">
+      <c r="K48" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="L48" s="4" t="n">
+      <c r="L48" s="1" t="n">
         <v>32612</v>
       </c>
-      <c r="M48" s="4" t="n">
+      <c r="M48" s="1" t="n">
         <v>2275</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C49" s="0" t="n">
@@ -2474,24 +2453,24 @@
       <c r="I49" s="0" t="n">
         <v>1595633</v>
       </c>
-      <c r="J49" s="4" t="n">
+      <c r="J49" s="1" t="n">
         <v>2274</v>
       </c>
-      <c r="K49" s="4" t="n">
+      <c r="K49" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="L49" s="4" t="n">
+      <c r="L49" s="1" t="n">
         <v>32525</v>
       </c>
-      <c r="M49" s="4" t="n">
+      <c r="M49" s="1" t="n">
         <v>2225</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C50" s="0" t="n">
@@ -2515,24 +2494,24 @@
       <c r="I50" s="0" t="n">
         <v>1482730</v>
       </c>
-      <c r="J50" s="4" t="n">
+      <c r="J50" s="1" t="n">
         <v>2089</v>
       </c>
-      <c r="K50" s="4" t="n">
+      <c r="K50" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="L50" s="4" t="n">
+      <c r="L50" s="1" t="n">
         <v>31678</v>
       </c>
-      <c r="M50" s="4" t="n">
+      <c r="M50" s="1" t="n">
         <v>2803</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C51" s="0" t="n">
@@ -2556,24 +2535,24 @@
       <c r="I51" s="0" t="n">
         <v>1471463</v>
       </c>
-      <c r="J51" s="4" t="n">
+      <c r="J51" s="1" t="n">
         <v>1997</v>
       </c>
-      <c r="K51" s="4" t="n">
+      <c r="K51" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="L51" s="4" t="n">
+      <c r="L51" s="1" t="n">
         <v>30781</v>
       </c>
-      <c r="M51" s="4" t="n">
+      <c r="M51" s="1" t="n">
         <v>2773</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C52" s="0" t="n">
@@ -2597,24 +2576,24 @@
       <c r="I52" s="0" t="n">
         <v>1207745</v>
       </c>
-      <c r="J52" s="4" t="n">
+      <c r="J52" s="1" t="n">
         <v>1634</v>
       </c>
-      <c r="K52" s="4" t="n">
+      <c r="K52" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="L52" s="4" t="n">
+      <c r="L52" s="1" t="n">
         <v>29801</v>
       </c>
-      <c r="M52" s="4" t="n">
+      <c r="M52" s="1" t="n">
         <v>2497</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C53" s="0" t="n">
@@ -2638,24 +2617,24 @@
       <c r="I53" s="0" t="n">
         <v>1253313</v>
       </c>
-      <c r="J53" s="4" t="n">
+      <c r="J53" s="1" t="n">
         <v>1972</v>
       </c>
-      <c r="K53" s="4" t="n">
+      <c r="K53" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="L53" s="4" t="n">
+      <c r="L53" s="1" t="n">
         <v>28495</v>
       </c>
-      <c r="M53" s="4" t="n">
+      <c r="M53" s="1" t="n">
         <v>3156</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C54" s="0" t="n">
@@ -2679,24 +2658,24 @@
       <c r="I54" s="0" t="n">
         <v>1749433</v>
       </c>
-      <c r="J54" s="4" t="n">
+      <c r="J54" s="1" t="n">
         <v>1837</v>
       </c>
-      <c r="K54" s="4" t="n">
+      <c r="K54" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="L54" s="4" t="n">
+      <c r="L54" s="1" t="n">
         <v>23725</v>
       </c>
-      <c r="M54" s="4" t="n">
+      <c r="M54" s="1" t="n">
         <v>6482</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>82</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C55" s="0" t="n">
@@ -2720,24 +2699,24 @@
       <c r="I55" s="0" t="n">
         <v>1874748</v>
       </c>
-      <c r="J55" s="4" t="n">
+      <c r="J55" s="1" t="n">
         <v>1657</v>
       </c>
-      <c r="K55" s="4" t="n">
+      <c r="K55" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="L55" s="4" t="n">
+      <c r="L55" s="1" t="n">
         <v>23318</v>
       </c>
-      <c r="M55" s="4" t="n">
+      <c r="M55" s="1" t="n">
         <v>1947</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C56" s="0" t="n">
@@ -2761,24 +2740,24 @@
       <c r="I56" s="0" t="n">
         <v>1907096</v>
       </c>
-      <c r="J56" s="4" t="n">
+      <c r="J56" s="1" t="n">
         <v>1617</v>
       </c>
-      <c r="K56" s="4" t="n">
+      <c r="K56" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="L56" s="4" t="n">
+      <c r="L56" s="1" t="n">
         <v>22735</v>
       </c>
-      <c r="M56" s="4" t="n">
+      <c r="M56" s="1" t="n">
         <v>2089</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C57" s="0" t="n">
@@ -2802,24 +2781,24 @@
       <c r="I57" s="0" t="n">
         <v>1944695</v>
       </c>
-      <c r="J57" s="4" t="n">
+      <c r="J57" s="1" t="n">
         <v>1574</v>
       </c>
-      <c r="K57" s="4" t="n">
+      <c r="K57" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="L57" s="4" t="n">
+      <c r="L57" s="1" t="n">
         <v>22065</v>
       </c>
-      <c r="M57" s="4" t="n">
+      <c r="M57" s="1" t="n">
         <v>2146</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C58" s="0" t="n">
@@ -2843,24 +2822,24 @@
       <c r="I58" s="0" t="n">
         <v>2047846</v>
       </c>
-      <c r="J58" s="4" t="n">
+      <c r="J58" s="1" t="n">
         <v>1512</v>
       </c>
-      <c r="K58" s="4" t="n">
+      <c r="K58" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="L58" s="4" t="n">
+      <c r="L58" s="1" t="n">
         <v>21679</v>
       </c>
-      <c r="M58" s="4" t="n">
+      <c r="M58" s="1" t="n">
         <v>1804</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C59" s="0" t="n">
@@ -2884,24 +2863,24 @@
       <c r="I59" s="0" t="n">
         <v>2005994</v>
       </c>
-      <c r="J59" s="4" t="n">
+      <c r="J59" s="1" t="n">
         <v>1606</v>
       </c>
-      <c r="K59" s="4" t="n">
+      <c r="K59" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="L59" s="4" t="n">
+      <c r="L59" s="1" t="n">
         <v>20897</v>
       </c>
-      <c r="M59" s="4" t="n">
+      <c r="M59" s="1" t="n">
         <v>2296</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C60" s="0" t="n">
@@ -2925,24 +2904,24 @@
       <c r="I60" s="0" t="n">
         <v>1779050</v>
       </c>
-      <c r="J60" s="4" t="n">
+      <c r="J60" s="1" t="n">
         <v>1499</v>
       </c>
-      <c r="K60" s="4" t="n">
+      <c r="K60" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="L60" s="4" t="n">
+      <c r="L60" s="1" t="n">
         <v>20472</v>
       </c>
-      <c r="M60" s="4" t="n">
+      <c r="M60" s="1" t="n">
         <v>1835</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C61" s="0" t="n">
@@ -2966,24 +2945,24 @@
       <c r="I61" s="0" t="n">
         <v>2162290</v>
       </c>
-      <c r="J61" s="4" t="n">
+      <c r="J61" s="1" t="n">
         <v>1374</v>
       </c>
-      <c r="K61" s="4" t="n">
+      <c r="K61" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="L61" s="4" t="n">
+      <c r="L61" s="1" t="n">
         <v>19850</v>
       </c>
-      <c r="M61" s="4" t="n">
+      <c r="M61" s="1" t="n">
         <v>1923</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>89</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="0" t="n">
@@ -3007,24 +2986,24 @@
       <c r="I62" s="0" t="n">
         <v>2184415</v>
       </c>
-      <c r="J62" s="4" t="n">
+      <c r="J62" s="1" t="n">
         <v>1343</v>
       </c>
-      <c r="K62" s="4" t="n">
+      <c r="K62" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="L62" s="4" t="n">
+      <c r="L62" s="1" t="n">
         <v>20070</v>
       </c>
-      <c r="M62" s="4" t="n">
+      <c r="M62" s="1" t="n">
         <v>1036</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C63" s="0" t="n">
@@ -3048,24 +3027,24 @@
       <c r="I63" s="0" t="n">
         <v>2324678</v>
       </c>
-      <c r="J63" s="4" t="n">
+      <c r="J63" s="1" t="n">
         <v>1294</v>
       </c>
-      <c r="K63" s="4" t="n">
+      <c r="K63" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="L63" s="4" t="n">
+      <c r="L63" s="1" t="n">
         <v>19023</v>
       </c>
-      <c r="M63" s="4" t="n">
+      <c r="M63" s="1" t="n">
         <v>2250</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="0" t="n">
@@ -3089,24 +3068,24 @@
       <c r="I64" s="0" t="n">
         <v>2309783</v>
       </c>
-      <c r="J64" s="4" t="n">
+      <c r="J64" s="1" t="n">
         <v>1297</v>
       </c>
-      <c r="K64" s="4" t="n">
+      <c r="K64" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="L64" s="4" t="n">
+      <c r="L64" s="1" t="n">
         <v>18540</v>
       </c>
-      <c r="M64" s="4" t="n">
+      <c r="M64" s="1" t="n">
         <v>1692</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="0" t="n">
@@ -3130,24 +3109,24 @@
       <c r="I65" s="0" t="n">
         <v>2405764</v>
       </c>
-      <c r="J65" s="4" t="n">
+      <c r="J65" s="1" t="n">
         <v>1194</v>
       </c>
-      <c r="K65" s="4" t="n">
+      <c r="K65" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="L65" s="4" t="n">
+      <c r="L65" s="1" t="n">
         <v>17492</v>
       </c>
-      <c r="M65" s="4" t="n">
+      <c r="M65" s="1" t="n">
         <v>2148</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C66" s="0" t="n">
@@ -3171,24 +3150,24 @@
       <c r="I66" s="0" t="n">
         <v>2287171</v>
       </c>
-      <c r="J66" s="4" t="n">
+      <c r="J66" s="1" t="n">
         <v>1030</v>
       </c>
-      <c r="K66" s="4" t="n">
+      <c r="K66" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="L66" s="4" t="n">
+      <c r="L66" s="1" t="n">
         <v>16702</v>
       </c>
-      <c r="M66" s="4" t="n">
+      <c r="M66" s="1" t="n">
         <v>1730</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>94</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C67" s="0" t="n">
@@ -3212,24 +3191,24 @@
       <c r="I67" s="0" t="n">
         <v>2090121</v>
       </c>
-      <c r="J67" s="4" t="n">
+      <c r="J67" s="1" t="n">
         <v>1168</v>
       </c>
-      <c r="K67" s="4" t="n">
+      <c r="K67" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="L67" s="4" t="n">
+      <c r="L67" s="1" t="n">
         <v>16021</v>
       </c>
-      <c r="M67" s="4" t="n">
+      <c r="M67" s="1" t="n">
         <v>1756</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C68" s="0" t="n">
@@ -3253,24 +3232,24 @@
       <c r="I68" s="0" t="n">
         <v>2379302</v>
       </c>
-      <c r="J68" s="4" t="n">
+      <c r="J68" s="1" t="n">
         <v>1134</v>
       </c>
-      <c r="K68" s="4" t="n">
+      <c r="K68" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="L68" s="4" t="n">
+      <c r="L68" s="1" t="n">
         <v>15485</v>
       </c>
-      <c r="M68" s="4" t="n">
+      <c r="M68" s="1" t="n">
         <v>1594</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C69" s="0" t="n">
@@ -3294,24 +3273,24 @@
       <c r="I69" s="0" t="n">
         <v>2208686</v>
       </c>
-      <c r="J69" s="4" t="n">
+      <c r="J69" s="1" t="n">
         <v>1153</v>
       </c>
-      <c r="K69" s="4" t="n">
+      <c r="K69" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="L69" s="4" t="n">
+      <c r="L69" s="1" t="n">
         <v>15114</v>
       </c>
-      <c r="M69" s="4" t="n">
+      <c r="M69" s="1" t="n">
         <v>1464</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>97</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C70" s="0" t="n">
@@ -3335,24 +3314,24 @@
       <c r="I70" s="0" t="n">
         <v>2304837</v>
       </c>
-      <c r="J70" s="4" t="n">
+      <c r="J70" s="1" t="n">
         <v>991</v>
       </c>
-      <c r="K70" s="4" t="n">
+      <c r="K70" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="L70" s="4" t="n">
+      <c r="L70" s="1" t="n">
         <v>14733</v>
       </c>
-      <c r="M70" s="4" t="n">
+      <c r="M70" s="1" t="n">
         <v>1276</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C71" s="0" t="n">
@@ -3376,24 +3355,24 @@
       <c r="I71" s="0" t="n">
         <v>2306042</v>
       </c>
-      <c r="J71" s="4" t="n">
+      <c r="J71" s="1" t="n">
         <v>1112</v>
       </c>
-      <c r="K71" s="4" t="n">
+      <c r="K71" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="L71" s="4" t="n">
+      <c r="L71" s="1" t="n">
         <v>14268</v>
       </c>
-      <c r="M71" s="4" t="n">
+      <c r="M71" s="1" t="n">
         <v>1506</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C72" s="0" t="n">
@@ -3417,24 +3396,24 @@
       <c r="I72" s="0" t="n">
         <v>2474824</v>
       </c>
-      <c r="J72" s="4" t="n">
+      <c r="J72" s="1" t="n">
         <v>1073</v>
       </c>
-      <c r="K72" s="4" t="n">
+      <c r="K72" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="L72" s="4" t="n">
+      <c r="L72" s="1" t="n">
         <v>13909</v>
       </c>
-      <c r="M72" s="4" t="n">
+      <c r="M72" s="1" t="n">
         <v>1352</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C73" s="0" t="n">
@@ -3458,24 +3437,24 @@
       <c r="I73" s="0" t="n">
         <v>2405902</v>
       </c>
-      <c r="J73" s="4" t="n">
+      <c r="J73" s="1" t="n">
         <v>983</v>
       </c>
-      <c r="K73" s="4" t="n">
+      <c r="K73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="L73" s="4" t="n">
+      <c r="L73" s="1" t="n">
         <v>13509</v>
       </c>
-      <c r="M73" s="4" t="n">
+      <c r="M73" s="1" t="n">
         <v>1312</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C74" s="0" t="n">
@@ -3499,24 +3478,24 @@
       <c r="I74" s="0" t="n">
         <v>2244131</v>
       </c>
-      <c r="J74" s="4" t="n">
+      <c r="J74" s="1" t="n">
         <v>1006</v>
       </c>
-      <c r="K74" s="4" t="n">
+      <c r="K74" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="L74" s="4" t="n">
+      <c r="L74" s="1" t="n">
         <v>13237</v>
       </c>
-      <c r="M74" s="4" t="n">
+      <c r="M74" s="1" t="n">
         <v>1215</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C75" s="0" t="n">
@@ -3540,24 +3519,24 @@
       <c r="I75" s="0" t="n">
         <v>2579753</v>
       </c>
-      <c r="J75" s="4" t="n">
+      <c r="J75" s="1" t="n">
         <v>802</v>
       </c>
-      <c r="K75" s="4" t="n">
+      <c r="K75" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="L75" s="4" t="n">
+      <c r="L75" s="1" t="n">
         <v>12942</v>
       </c>
-      <c r="M75" s="4" t="n">
+      <c r="M75" s="1" t="n">
         <v>1032</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>103</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C76" s="0" t="n">
@@ -3581,24 +3560,24 @@
       <c r="I76" s="0" t="n">
         <v>2476314</v>
       </c>
-      <c r="J76" s="4" t="n">
+      <c r="J76" s="1" t="n">
         <v>976</v>
       </c>
-      <c r="K76" s="4" t="n">
+      <c r="K76" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="L76" s="4" t="n">
+      <c r="L76" s="1" t="n">
         <v>12799</v>
       </c>
-      <c r="M76" s="4" t="n">
+      <c r="M76" s="1" t="n">
         <v>1072</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>104</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C77" s="0" t="n">
@@ -3622,24 +3601,24 @@
       <c r="I77" s="0" t="n">
         <v>2527712</v>
       </c>
-      <c r="J77" s="4" t="n">
+      <c r="J77" s="1" t="n">
         <v>1223</v>
       </c>
-      <c r="K77" s="4" t="n">
+      <c r="K77" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="L77" s="4" t="n">
+      <c r="L77" s="1" t="n">
         <v>12991</v>
       </c>
-      <c r="M77" s="4" t="n">
+      <c r="M77" s="1" t="n">
         <v>957</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>105</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C78" s="0" t="n">
@@ -3663,24 +3642,24 @@
       <c r="I78" s="0" t="n">
         <v>2571438</v>
       </c>
-      <c r="J78" s="4" t="n">
+      <c r="J78" s="1" t="n">
         <v>1323</v>
       </c>
-      <c r="K78" s="4" t="n">
+      <c r="K78" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="L78" s="4" t="n">
+      <c r="L78" s="1" t="n">
         <v>13155</v>
       </c>
-      <c r="M78" s="4" t="n">
+      <c r="M78" s="1" t="n">
         <v>1096</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>106</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C79" s="0" t="n">
@@ -3704,24 +3683,24 @@
       <c r="I79" s="0" t="n">
         <v>2640331</v>
       </c>
-      <c r="J79" s="4" t="n">
+      <c r="J79" s="1" t="n">
         <v>1680</v>
       </c>
-      <c r="K79" s="4" t="n">
+      <c r="K79" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="L79" s="4" t="n">
+      <c r="L79" s="1" t="n">
         <v>13645</v>
       </c>
-      <c r="M79" s="4" t="n">
+      <c r="M79" s="1" t="n">
         <v>1112</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C80" s="0" t="n">
@@ -3745,24 +3724,24 @@
       <c r="I80" s="0" t="n">
         <v>2609841</v>
       </c>
-      <c r="J80" s="4" t="n">
+      <c r="J80" s="1" t="n">
         <v>1485</v>
       </c>
-      <c r="K80" s="4" t="n">
+      <c r="K80" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="L80" s="4" t="n">
+      <c r="L80" s="1" t="n">
         <v>13905</v>
       </c>
-      <c r="M80" s="4" t="n">
+      <c r="M80" s="1" t="n">
         <v>1157</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>108</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C81" s="0" t="n">
@@ -3786,24 +3765,24 @@
       <c r="I81" s="0" t="n">
         <v>2409207</v>
       </c>
-      <c r="J81" s="4" t="n">
+      <c r="J81" s="1" t="n">
         <v>1556</v>
       </c>
-      <c r="K81" s="4" t="n">
+      <c r="K81" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="L81" s="4" t="n">
+      <c r="L81" s="1" t="n">
         <v>14313</v>
       </c>
-      <c r="M81" s="4" t="n">
+      <c r="M81" s="1" t="n">
         <v>1093</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>109</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C82" s="0" t="n">
@@ -3827,24 +3806,24 @@
       <c r="I82" s="0" t="n">
         <v>2661421</v>
       </c>
-      <c r="J82" s="4" t="n">
+      <c r="J82" s="1" t="n">
         <v>1529</v>
       </c>
-      <c r="K82" s="4" t="n">
+      <c r="K82" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="L82" s="4" t="n">
+      <c r="L82" s="1" t="n">
         <v>14567</v>
       </c>
-      <c r="M82" s="4" t="n">
+      <c r="M82" s="1" t="n">
         <v>1227</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C83" s="0" t="n">
@@ -3868,24 +3847,24 @@
       <c r="I83" s="0" t="n">
         <v>2507040</v>
       </c>
-      <c r="J83" s="4" t="n">
+      <c r="J83" s="1" t="n">
         <v>1383</v>
       </c>
-      <c r="K83" s="4" t="n">
+      <c r="K83" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="L83" s="4" t="n">
+      <c r="L83" s="1" t="n">
         <v>14820</v>
       </c>
-      <c r="M83" s="4" t="n">
+      <c r="M83" s="1" t="n">
         <v>1079</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>111</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C84" s="0" t="n">
@@ -3909,24 +3888,24 @@
       <c r="I84" s="0" t="n">
         <v>2506211</v>
       </c>
-      <c r="J84" s="4" t="n">
+      <c r="J84" s="1" t="n">
         <v>1683</v>
       </c>
-      <c r="K84" s="4" t="n">
+      <c r="K84" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="L84" s="4" t="n">
+      <c r="L84" s="1" t="n">
         <v>15179</v>
       </c>
-      <c r="M84" s="4" t="n">
+      <c r="M84" s="1" t="n">
         <v>1279</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>112</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C85" s="0" t="n">
@@ -3950,24 +3929,24 @@
       <c r="I85" s="0" t="n">
         <v>2494855</v>
       </c>
-      <c r="J85" s="4" t="n">
+      <c r="J85" s="1" t="n">
         <v>1481</v>
       </c>
-      <c r="K85" s="4" t="n">
+      <c r="K85" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="L85" s="4" t="n">
+      <c r="L85" s="1" t="n">
         <v>15677</v>
       </c>
-      <c r="M85" s="4" t="n">
+      <c r="M85" s="1" t="n">
         <v>935</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>113</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C86" s="0" t="n">
@@ -3991,24 +3970,24 @@
       <c r="I86" s="0" t="n">
         <v>2525600</v>
       </c>
-      <c r="J86" s="4" t="n">
+      <c r="J86" s="1" t="n">
         <v>1958</v>
       </c>
-      <c r="K86" s="4" t="n">
+      <c r="K86" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="L86" s="4" t="n">
+      <c r="L86" s="1" t="n">
         <v>16514</v>
       </c>
-      <c r="M86" s="4" t="n">
+      <c r="M86" s="1" t="n">
         <v>1071</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C87" s="0" t="n">
@@ -4032,24 +4011,24 @@
       <c r="I87" s="0" t="n">
         <v>2494118</v>
       </c>
-      <c r="J87" s="4" t="n">
+      <c r="J87" s="1" t="n">
         <v>1808</v>
       </c>
-      <c r="K87" s="4" t="n">
+      <c r="K87" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="L87" s="4" t="n">
+      <c r="L87" s="1" t="n">
         <v>17140</v>
       </c>
-      <c r="M87" s="4" t="n">
+      <c r="M87" s="1" t="n">
         <v>1111</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C88" s="0" t="n">
@@ -4073,24 +4052,24 @@
       <c r="I88" s="0" t="n">
         <v>2124248</v>
       </c>
-      <c r="J88" s="4" t="n">
+      <c r="J88" s="1" t="n">
         <v>2102</v>
       </c>
-      <c r="K88" s="4" t="n">
+      <c r="K88" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="L88" s="4" t="n">
+      <c r="L88" s="1" t="n">
         <v>17897</v>
       </c>
-      <c r="M88" s="4" t="n">
+      <c r="M88" s="1" t="n">
         <v>1297</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C89" s="0" t="n">
@@ -4114,24 +4093,24 @@
       <c r="I89" s="0" t="n">
         <v>2599034</v>
       </c>
-      <c r="J89" s="4" t="n">
+      <c r="J89" s="1" t="n">
         <v>1757</v>
       </c>
-      <c r="K89" s="4" t="n">
+      <c r="K89" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="L89" s="4" t="n">
+      <c r="L89" s="1" t="n">
         <v>18308</v>
       </c>
-      <c r="M89" s="4" t="n">
+      <c r="M89" s="1" t="n">
         <v>1311</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>117</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C90" s="0" t="n">
@@ -4155,24 +4134,24 @@
       <c r="I90" s="0" t="n">
         <v>2525795</v>
       </c>
-      <c r="J90" s="4" t="n">
+      <c r="J90" s="1" t="n">
         <v>1806</v>
       </c>
-      <c r="K90" s="4" t="n">
+      <c r="K90" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="L90" s="4" t="n">
+      <c r="L90" s="1" t="n">
         <v>18746</v>
       </c>
-      <c r="M90" s="4" t="n">
+      <c r="M90" s="1" t="n">
         <v>1317</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C91" s="0" t="n">
@@ -4196,24 +4175,24 @@
       <c r="I91" s="0" t="n">
         <v>2583446</v>
       </c>
-      <c r="J91" s="4" t="n">
+      <c r="J91" s="1" t="n">
         <v>2294</v>
       </c>
-      <c r="K91" s="4" t="n">
+      <c r="K91" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="L91" s="4" t="n">
+      <c r="L91" s="1" t="n">
         <v>19774</v>
       </c>
-      <c r="M91" s="4" t="n">
+      <c r="M91" s="1" t="n">
         <v>1197</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C92" s="0" t="n">
@@ -4237,24 +4216,24 @@
       <c r="I92" s="0" t="n">
         <v>2581506</v>
       </c>
-      <c r="J92" s="4" t="n">
+      <c r="J92" s="1" t="n">
         <v>2111</v>
       </c>
-      <c r="K92" s="4" t="n">
+      <c r="K92" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="L92" s="4" t="n">
+      <c r="L92" s="1" t="n">
         <v>20311</v>
       </c>
-      <c r="M92" s="4" t="n">
+      <c r="M92" s="1" t="n">
         <v>1512</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C93" s="0" t="n">
@@ -4278,16 +4257,16 @@
       <c r="I93" s="0" t="n">
         <v>2690453</v>
       </c>
-      <c r="J93" s="4" t="n">
+      <c r="J93" s="1" t="n">
         <v>2346</v>
       </c>
-      <c r="K93" s="4" t="n">
+      <c r="K93" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="L93" s="4" t="n">
+      <c r="L93" s="1" t="n">
         <v>20958</v>
       </c>
-      <c r="M93" s="4" t="n">
+      <c r="M93" s="1" t="n">
         <v>1635</v>
       </c>
     </row>

</xml_diff>